<commit_message>
fully fleshed out the excel spreadsheet to aid in calculating values
</commit_message>
<xml_diff>
--- a/stat-calculator.xlsx
+++ b/stat-calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\Event Horizon 1.9.1 build 1394 (database testing)\Mods\Event-Horizon-ES-mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E5583-478B-4842-8386-6FEF4169B0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE8F96-3966-4E55-911E-8FD587209DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
   </bookViews>
@@ -36,29 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Source</t>
   </si>
   <si>
-    <t>In-Game</t>
-  </si>
-  <si>
     <t>In-Mod</t>
   </si>
   <si>
     <t>Armor Regen</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>Energy Regen</t>
   </si>
   <si>
-    <t>Shield</t>
-  </si>
-  <si>
     <t>Shield Regen</t>
   </si>
   <si>
@@ -68,18 +59,9 @@
     <t>Turning Power</t>
   </si>
   <si>
-    <t>Ion Thrust</t>
-  </si>
-  <si>
-    <t>Ion Turn</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Damage (Shield + Hull)</t>
-  </si>
-  <si>
     <t>Projectiles</t>
   </si>
   <si>
@@ -89,15 +71,6 @@
     <t>Lasers</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>x2 boost for syscores</t>
-  </si>
-  <si>
-    <t>Heat (sum)</t>
-  </si>
-  <si>
     <t>/250 for normal modules, /500 for some active coolers</t>
   </si>
   <si>
@@ -107,10 +80,91 @@
     <t>Energy Cost (per shot)</t>
   </si>
   <si>
-    <t>Divide superweapons by 100</t>
-  </si>
-  <si>
-    <t>Divide ions by 20</t>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>See C15</t>
+  </si>
+  <si>
+    <t>/10 for missiles instead of 50</t>
+  </si>
+  <si>
+    <t>x2 for system cores and bird reactors</t>
+  </si>
+  <si>
+    <t>/100 for superweapons, /20 for ions (/50 for strong ions)</t>
+  </si>
+  <si>
+    <t>Modifier Notes (replaces default modifiers)</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>"In-game" describes shots/s</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>See C11</t>
+  </si>
+  <si>
+    <t>Divide by 5</t>
+  </si>
+  <si>
+    <t>See D5</t>
+  </si>
+  <si>
+    <t>In-Game (calculated)</t>
+  </si>
+  <si>
+    <t>In-Game (encyclopedia)</t>
+  </si>
+  <si>
+    <t>PUOS (encyclopedia)</t>
+  </si>
+  <si>
+    <t>In-Mod (pedia)</t>
+  </si>
+  <si>
+    <t>See E3/E4</t>
+  </si>
+  <si>
+    <t>Never set size to 0</t>
+  </si>
+  <si>
+    <t>Energy Cost (sum)</t>
+  </si>
+  <si>
+    <t>Heat / Cooling (sum)</t>
+  </si>
+  <si>
+    <t>10% of G6</t>
+  </si>
+  <si>
+    <t>minus 20% for systems cores</t>
+  </si>
+  <si>
+    <t>Energy Storage</t>
+  </si>
+  <si>
+    <t>Shield HP</t>
+  </si>
+  <si>
+    <t>In-game (calculated)</t>
+  </si>
+  <si>
+    <t>In-game (encyclopedia)</t>
+  </si>
+  <si>
+    <t>Damage (continuous)</t>
+  </si>
+  <si>
+    <t>Damage (per shot)</t>
+  </si>
+  <si>
+    <t>See B17</t>
   </si>
 </sst>
 </file>
@@ -462,42 +516,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090DF3EA-211C-4B44-95A2-4E20E8C2A341}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -506,17 +572,32 @@
         <f>IMPRODUCT(60, B2)</f>
         <v>0</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
         <f>IMDIV(C2, B10)</f>
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>IMDIV(D2,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IMPRODUCT(E2, 1/250)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IMPRODUCT(F2, 1/250)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -525,33 +606,61 @@
         <f>IMPRODUCT(60,B3)</f>
         <v>0</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
         <f>IMDIV(C3, B10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f>IMDIV(D3,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="str">
-        <f>IMPRODUCT(B4, 60)</f>
-        <v>0</v>
-      </c>
-      <c r="D4" t="str">
-        <f>IMDIV(C4/B10,10)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f>IMPRODUCT(B4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IMDIV(C4, B10)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" t="str">
+        <f>IMDIV(D4,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IMPRODUCT(E4,1/10)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <f>IMPRODUCT(F4,1/10)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -560,14 +669,30 @@
         <f>IMPRODUCT(B5, 60)</f>
         <v>0</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
         <f>IMDIV(C5, B10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f>IMDIV(D5,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -576,10 +701,29 @@
         <f>IMPRODUCT(B6, 60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IMDIV(C6,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <f>IMDIV(D6,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IMPRODUCT(E6,5)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IMPRODUCT(F6,5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -588,14 +732,24 @@
         <f>IMPRODUCT(B7, 60)</f>
         <v>0</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
         <f>IMDIV(C7, B10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f>IMDIV(D7,B10)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -604,10 +758,17 @@
         <f>IMPRODUCT(B8, 60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <f>IMDIV(D8,B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -616,70 +777,183 @@
         <f>IMPRODUCT(B9, 3600)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <f>IMDIV(D9,B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f>IMPRODUCT(B11,1/10)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="str">
+        <f>IMDIV(D12,B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>15.6</v>
+      </c>
+      <c r="C15" t="str">
+        <f>IMPRODUCT(B15,60)</f>
+        <v>936</v>
+      </c>
+      <c r="E15" t="str">
+        <f>IMPRODUCT(B17,1/10)</f>
+        <v>552</v>
+      </c>
+      <c r="F15" t="str">
+        <f>IMPRODUCT(B17,1/20)</f>
+        <v>276</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IMPRODUCT(C15,1/15)</f>
+        <v>62.4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+      <c r="C16" t="str">
+        <f>IMPRODUCT(B16,60)</f>
+        <v>150</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IMPRODUCT(C16,1/10)</f>
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>5520</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <f>IMPRODUCT(B18,1/10)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" t="str">
+        <f>IMPRODUCT(B18,1/50)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" t="str">
-        <f>IMPRODUCT(B14,1/10)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" t="str">
-        <f>IMPRODUCT(B14,1/20)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" t="str">
-        <f>IMPRODUCT(B14,1/15)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user-side changes to a couple of things that won't matter for anyone forking or cloning this repo
</commit_message>
<xml_diff>
--- a/stat-calculator.xlsx
+++ b/stat-calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\Event Horizon 1.9.1 build 1394 (database testing)\Mods\Event-Horizon-ES-mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\EH 1.9.1 1394\Mods\Event-Horizon-ES-mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92111184-33A3-4E73-9A0E-96FB88310A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDEF358-9CFE-49A4-8FF9-385AF6F48EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,11 +869,11 @@
         <v>40</v>
       </c>
       <c r="B15">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="str">
         <f>IMPRODUCT(B15,60)</f>
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="E15" t="str">
         <f>IMPRODUCT(B17,1/10)</f>
@@ -885,7 +885,7 @@
       </c>
       <c r="G15" t="str">
         <f>IMPRODUCT(C15,1/15)</f>
-        <v>22.8</v>
+        <v>24</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
used calculator to check my math
</commit_message>
<xml_diff>
--- a/stat-calculator.xlsx
+++ b/stat-calculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\EH 1.9.1 1394\Mods\Event-Horizon-ES-mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA635ACD-1455-4A1E-B5CF-F917A080CDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08624A8A-67EF-4625-BF72-24DB7867E14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,18 +566,18 @@
         <v>33</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C2" t="str">
         <f>IMPRODUCT(60, B2)</f>
-        <v>0</v>
+        <v>1620</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>IMDIV(C2, B10)</f>
-        <v>0</v>
+        <v>25.7142857142857</v>
       </c>
       <c r="F2" t="str">
         <f>IMDIV(D2,B10)</f>
@@ -585,7 +585,7 @@
       </c>
       <c r="G2" t="str">
         <f>IMPRODUCT(E2, 1/250)</f>
-        <v>0</v>
+        <v>0.102857142857143</v>
       </c>
       <c r="H2" t="str">
         <f>IMPRODUCT(F2, 1/250)</f>
@@ -663,18 +663,18 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="C5" t="str">
         <f>IMPRODUCT(B5, 60)</f>
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="str">
         <f>IMDIV(C5, B10)</f>
-        <v>0</v>
+        <v>5.80952380952381</v>
       </c>
       <c r="F5" t="str">
         <f>IMDIV(D5,B10)</f>
@@ -790,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
removed a number of files (versions go to a new repo and database editor files to outside of repo
</commit_message>
<xml_diff>
--- a/stat-calculator.xlsx
+++ b/stat-calculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\EH 1.9.1 1394\Mods\Event-Horizon-ES-mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\EH 1.9.1 1394\Mods\Event-Horizon-ES-Mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08624A8A-67EF-4625-BF72-24DB7867E14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1AF30-3D98-434E-AA49-E24E75001709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Source</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Divide by 5</t>
   </si>
   <si>
-    <t>See D5</t>
-  </si>
-  <si>
     <t>In-Game (calculated)</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Heat / Cooling (sum)</t>
   </si>
   <si>
-    <t>10% of G6</t>
-  </si>
-  <si>
     <t>minus 20% for systems cores</t>
   </si>
   <si>
@@ -165,6 +159,9 @@
   </si>
   <si>
     <t>See B17</t>
+  </si>
+  <si>
+    <t>E5</t>
   </si>
 </sst>
 </file>
@@ -519,7 +516,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,22 +537,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
@@ -563,21 +560,21 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C2" t="str">
         <f>IMPRODUCT(60, B2)</f>
-        <v>1620</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>IMDIV(C2, B10)</f>
-        <v>25.7142857142857</v>
+        <v>0</v>
       </c>
       <c r="F2" t="str">
         <f>IMDIV(D2,B10)</f>
@@ -585,7 +582,7 @@
       </c>
       <c r="G2" t="str">
         <f>IMPRODUCT(E2, 1/250)</f>
-        <v>0.102857142857143</v>
+        <v>0</v>
       </c>
       <c r="H2" t="str">
         <f>IMPRODUCT(F2, 1/250)</f>
@@ -618,15 +615,15 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -663,50 +660,51 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C5" t="str">
         <f>IMPRODUCT(B5, 60)</f>
-        <v>366</v>
+        <v>264</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="str">
         <f>IMDIV(C5, B10)</f>
-        <v>5.80952380952381</v>
+        <v>1.73684210526316</v>
       </c>
       <c r="F5" t="str">
         <f>IMDIV(D5,B10)</f>
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>25</v>
+      <c r="G5" t="str">
+        <f>E5</f>
+        <v>1.73684210526316</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C6" t="str">
         <f>IMPRODUCT(B6, 60)</f>
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="str">
         <f>IMDIV(C6,B10)</f>
-        <v>0</v>
+        <v>1.73684210526316</v>
       </c>
       <c r="F6" t="str">
         <f>IMDIV(D6,B10)</f>
@@ -714,7 +712,7 @@
       </c>
       <c r="G6" t="str">
         <f>IMPRODUCT(E6,5)</f>
-        <v>0</v>
+        <v>8.6842105263158</v>
       </c>
       <c r="H6" t="str">
         <f>IMPRODUCT(F6,5)</f>
@@ -743,8 +741,9 @@
         <f>IMDIV(D7,B10)</f>
         <v>0</v>
       </c>
-      <c r="G7" t="s">
-        <v>34</v>
+      <c r="G7" t="str">
+        <f>IMPRODUCT(G6,0.1)</f>
+        <v>0.86842105263158</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -752,14 +751,18 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>207.7</v>
       </c>
       <c r="C8" t="str">
-        <f>IMPRODUCT(B8, 60)</f>
-        <v>0</v>
+        <f>IMPRODUCT(B8, 3600)</f>
+        <v>747720</v>
       </c>
       <c r="D8">
         <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f>IMDIV(C8, B10)</f>
+        <v>4919.21052631579</v>
       </c>
       <c r="F8" t="str">
         <f>IMDIV(D8,B10)</f>
@@ -771,14 +774,18 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>5010</v>
       </c>
       <c r="C9" t="str">
-        <f>IMPRODUCT(B9, 3600)</f>
-        <v>0</v>
+        <f>IMPRODUCT(B9,60)</f>
+        <v>300600</v>
       </c>
       <c r="D9">
         <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <f>IMDIV(C9, B10)</f>
+        <v>1977.63157894737</v>
       </c>
       <c r="F9" t="str">
         <f>IMDIV(D9,B10)</f>
@@ -790,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -811,7 +818,7 @@
         <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -834,7 +841,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -849,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -866,14 +873,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>10.199999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="C15" t="str">
         <f>IMPRODUCT(B15,60)</f>
-        <v>612</v>
+        <v>252</v>
       </c>
       <c r="E15" t="str">
         <f>IMPRODUCT(B17,1/10)</f>
@@ -885,7 +892,7 @@
       </c>
       <c r="G15" t="str">
         <f>IMPRODUCT(C15,1/15)</f>
-        <v>40.8</v>
+        <v>16.8</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -896,15 +903,15 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>2.5</v>
+        <v>4.87</v>
       </c>
       <c r="C16" t="str">
         <f>IMPRODUCT(B16,60)</f>
-        <v>150</v>
+        <v>292.2</v>
       </c>
       <c r="E16" t="str">
         <f>IMPRODUCT(C16,1/10)</f>
-        <v>15</v>
+        <v>29.22</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -915,13 +922,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>3400</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -929,15 +936,15 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>3600</v>
       </c>
       <c r="E18" t="str">
         <f>IMPRODUCT(B18,1/10)</f>
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="F18" t="str">
         <f>IMPRODUCT(B18,1/50)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
misc: updated kestrel tester and stat generating excel spreadsheet
</commit_message>
<xml_diff>
--- a/stat-calculator.xlsx
+++ b/stat-calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\EH Database\EH 1.9.1 1394\Mods\Event-Horizon-ES-Mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\OneDrive\Desktop\EH_Database\Mods\Event-Horizon-ES-Mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1AF30-3D98-434E-AA49-E24E75001709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C554FD-79BC-4451-8754-74AF3ABCB130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
+    <workbookView xWindow="11484" yWindow="0" windowWidth="11724" windowHeight="13056" xr2:uid="{67DBE6CA-64D5-4C55-9ABA-59F80FECF45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Source</t>
   </si>
@@ -162,19 +162,84 @@
   </si>
   <si>
     <t>E5</t>
+  </si>
+  <si>
+    <t>Thrust</t>
+  </si>
+  <si>
+    <t>Steering</t>
+  </si>
+  <si>
+    <t>Ion engine comparison</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Reference ion values</t>
+  </si>
+  <si>
+    <t>Total size</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>thrust</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>In-game</t>
+  </si>
+  <si>
+    <t>Engine push</t>
+  </si>
+  <si>
+    <t>Engine energy cost</t>
+  </si>
+  <si>
+    <t>Value per outfit space</t>
+  </si>
+  <si>
+    <t>energy cost</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>Active cooling nrg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,8 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -257,7 +325,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -363,7 +431,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -505,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,26 +581,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090DF3EA-211C-4B44-95A2-4E20E8C2A341}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -558,23 +626,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="C2" t="str">
         <f>IMPRODUCT(60, B2)</f>
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>IMDIV(C2, B10)</f>
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F2" t="str">
         <f>IMDIV(D2,B10)</f>
@@ -582,7 +650,7 @@
       </c>
       <c r="G2" t="str">
         <f>IMPRODUCT(E2, 1/250)</f>
-        <v>0</v>
+        <v>0.0018</v>
       </c>
       <c r="H2" t="str">
         <f>IMPRODUCT(F2, 1/250)</f>
@@ -592,7 +660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -621,31 +689,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>16850</v>
       </c>
       <c r="C4" t="str">
         <f>IMPRODUCT(B4, 1)</f>
-        <v>0</v>
+        <v>16850</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="str">
         <f>IMDIV(C4, B10)</f>
-        <v>0</v>
+        <v>337</v>
       </c>
       <c r="F4" t="str">
         <f>IMDIV(D4,B10)</f>
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <f>IMPRODUCT(E4,1/10)</f>
-        <v>0</v>
+        <f>IMPRODUCT(E4,1/40)</f>
+        <v>8.425</v>
       </c>
       <c r="H4" t="str">
         <f>IMPRODUCT(F4,1/10)</f>
@@ -655,23 +723,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4.4000000000000004</v>
+        <v>0.375</v>
       </c>
       <c r="C5" t="str">
         <f>IMPRODUCT(B5, 60)</f>
-        <v>264</v>
+        <v>22.5</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="str">
         <f>IMDIV(C5, B10)</f>
-        <v>1.73684210526316</v>
+        <v>0.45</v>
       </c>
       <c r="F5" t="str">
         <f>IMDIV(D5,B10)</f>
@@ -679,7 +747,7 @@
       </c>
       <c r="G5" t="str">
         <f>E5</f>
-        <v>1.73684210526316</v>
+        <v>0.45</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -688,23 +756,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6">
-        <v>4.4000000000000004</v>
+        <v>0.375</v>
       </c>
       <c r="C6" t="str">
         <f>IMPRODUCT(B6, 60)</f>
-        <v>264</v>
+        <v>22.5</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="str">
         <f>IMDIV(C6,B10)</f>
-        <v>1.73684210526316</v>
+        <v>0.45</v>
       </c>
       <c r="F6" t="str">
         <f>IMDIV(D6,B10)</f>
@@ -712,14 +780,17 @@
       </c>
       <c r="G6" t="str">
         <f>IMPRODUCT(E6,5)</f>
-        <v>8.6842105263158</v>
+        <v>2.25</v>
       </c>
       <c r="H6" t="str">
         <f>IMPRODUCT(F6,5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -743,61 +814,65 @@
       </c>
       <c r="G7" t="str">
         <f>IMPRODUCT(G6,0.1)</f>
-        <v>0.86842105263158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.225</v>
+      </c>
+      <c r="L7">
+        <f>G5/5</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>207.7</v>
+        <v>0</v>
       </c>
       <c r="C8" t="str">
         <f>IMPRODUCT(B8, 3600)</f>
-        <v>747720</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="str">
         <f>IMDIV(C8, B10)</f>
-        <v>4919.21052631579</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IMDIV(D8,B10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>5010</v>
+        <v>0</v>
       </c>
       <c r="C9" t="str">
         <f>IMPRODUCT(B9,60)</f>
-        <v>300600</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="str">
         <f>IMDIV(C9, B10)</f>
-        <v>1977.63157894737</v>
+        <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>IMDIV(D9,B10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -821,7 +896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -839,7 +914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -851,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -871,7 +946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -898,7 +973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -920,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -931,7 +1006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -950,7 +1025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -964,7 +1039,257 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:9">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <f>112+28.4</f>
+        <v>140.4</v>
+      </c>
+      <c r="C22">
+        <f>B22*3600</f>
+        <v>505440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1750</v>
+      </c>
+      <c r="C23">
+        <f>B23*60</f>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <f>3+8.8+2.3</f>
+        <v>14.100000000000001</v>
+      </c>
+      <c r="C24">
+        <f>B24*60</f>
+        <v>846.00000000000011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>505440</v>
+      </c>
+      <c r="C26">
+        <v>105000</v>
+      </c>
+      <c r="D26">
+        <v>156</v>
+      </c>
+      <c r="E26" t="str">
+        <f>IMDIV(IMSUM(B26,C26),D26)</f>
+        <v>3913.07692307692</v>
+      </c>
+      <c r="F26">
+        <v>1900.6</v>
+      </c>
+      <c r="G26" t="str">
+        <f>IMDIV(E26,F26)</f>
+        <v>2.05886400246076</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28">
+        <v>846</v>
+      </c>
+      <c r="D28">
+        <v>101</v>
+      </c>
+      <c r="E28" t="str">
+        <f>IMDIV(C28,D28)</f>
+        <v>8.37623762376238</v>
+      </c>
+      <c r="F28">
+        <v>2.63</v>
+      </c>
+      <c r="G28" t="str">
+        <f>IMDIV(E28,F28)</f>
+        <v>3.18488122576516</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>21600</v>
+      </c>
+      <c r="C31">
+        <v>9600</v>
+      </c>
+      <c r="D31">
+        <v>28</v>
+      </c>
+      <c r="E31" t="str">
+        <f>IMDIV(IMSUM(B31,C31),D31)</f>
+        <v>1114.28571428571</v>
+      </c>
+      <c r="F31">
+        <v>54</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IMDIV(F31,D31)</f>
+        <v>1.92857142857143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>42400</v>
+      </c>
+      <c r="C32">
+        <v>12420</v>
+      </c>
+      <c r="D32">
+        <v>47</v>
+      </c>
+      <c r="E32" t="str">
+        <f>IMDIV(IMSUM(B32,C32),D32)</f>
+        <v>1166.3829787234</v>
+      </c>
+      <c r="F32">
+        <v>102</v>
+      </c>
+      <c r="G32" t="str">
+        <f>IMDIV(F32,D32)</f>
+        <v>2.17021276595745</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>79560</v>
+      </c>
+      <c r="C33">
+        <v>35400</v>
+      </c>
+      <c r="D33">
+        <v>81</v>
+      </c>
+      <c r="E33" t="str">
+        <f>IMDIV(IMSUM(B33,C33),D33)</f>
+        <v>1419.25925925926</v>
+      </c>
+      <c r="F33">
+        <v>180</v>
+      </c>
+      <c r="G33" t="str">
+        <f>IMDIV(F33,D33)</f>
+        <v>2.22222222222222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>153000</v>
+      </c>
+      <c r="C34">
+        <v>67920</v>
+      </c>
+      <c r="D34">
+        <v>138</v>
+      </c>
+      <c r="E34" t="str">
+        <f>IMDIV(IMSUM(B34,C34),D34)</f>
+        <v>1600.86956521739</v>
+      </c>
+      <c r="F34">
+        <v>324</v>
+      </c>
+      <c r="G34" t="str">
+        <f>IMDIV(F34,D34)</f>
+        <v>2.34782608695652</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>293400</v>
+      </c>
+      <c r="C35">
+        <v>130440</v>
+      </c>
+      <c r="D35">
+        <v>223</v>
+      </c>
+      <c r="E35" t="str">
+        <f>IMDIV(IMSUM(B35,C35),D35)</f>
+        <v>1900.62780269058</v>
+      </c>
+      <c r="F35">
+        <v>588</v>
+      </c>
+      <c r="G35" t="str">
+        <f>IMDIV(F35,D35)</f>
+        <v>2.63677130044843</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>